<commit_message>
Major updates to program, new version
</commit_message>
<xml_diff>
--- a/out/production/QuestInput/Excel/ShopTraveler.xlsx
+++ b/out/production/QuestInput/Excel/ShopTraveler.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewashley/Documents/IdeaProjects/QuestInput/src/sample/CustomerFiles/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B3BD27-3B77-C147-839D-91B90EEADF7E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shop Traveler" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -88,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -236,44 +235,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -285,6 +284,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -576,14 +578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -602,323 +604,321 @@
         <v>6</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="20"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7"/>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="19"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="19"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="11"/>
+      <c r="A8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="15"/>
+      <c r="D8" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20"/>
       <c r="F8" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11"/>
+      <c r="A9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="13"/>
       <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="15"/>
+      <c r="D9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="20"/>
       <c r="F9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11"/>
+      <c r="A10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="13"/>
       <c r="C10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="15"/>
+      <c r="D10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="20"/>
       <c r="F10" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11"/>
+      <c r="A11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="13"/>
       <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="15"/>
+      <c r="D11" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20"/>
       <c r="F11" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="15"/>
+      <c r="D12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="20"/>
       <c r="F12" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="13"/>
       <c r="C13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="15"/>
+      <c r="D13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20"/>
       <c r="F13" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="11"/>
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13"/>
       <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="15"/>
+      <c r="D14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="20"/>
       <c r="F14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="11"/>
+      <c r="A15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="13"/>
       <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="15"/>
+      <c r="D15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="20"/>
       <c r="F15" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11"/>
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13"/>
       <c r="C16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="15"/>
+      <c r="D16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20"/>
       <c r="F16" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="22">
+      <c r="B17" s="13"/>
+      <c r="C17" s="10">
         <f>SUM(C8:C16)</f>
         <v>0</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="22">
+      <c r="B18" s="13"/>
+      <c r="C18" s="10">
         <f>C17*E2</f>
         <v>0</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A20:F26"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A18:B18"/>
@@ -935,14 +935,16 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -957,28 +959,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>